<commit_message>
fin du xhi deux
</commit_message>
<xml_diff>
--- a/Xhi-deux.xlsx
+++ b/Xhi-deux.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\remi.DESKTOP-UI81QOM\Desktop\COURS v14chu\6. Stat R analyse linguistique 23-24\COURS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\remi.DESKTOP-UI81QOM\Desktop\VERSIONS PROJETS TT\COURS v15chu\6. Stat R analyse linguistique 23-24\COURS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E163037B-5075-417C-AB4A-390C62EF5286}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{478FE272-CED0-4A26-B445-7DA846E846A6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -368,8 +368,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="B45" sqref="B45"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -646,7 +646,7 @@
         <v>2</v>
       </c>
       <c r="C25" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.35">
@@ -657,7 +657,7 @@
         <v>3</v>
       </c>
       <c r="C26" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.35">
@@ -668,7 +668,7 @@
         <v>2</v>
       </c>
       <c r="C27" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.35">
@@ -756,7 +756,7 @@
         <v>2</v>
       </c>
       <c r="C35" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.35">
@@ -844,7 +844,7 @@
         <v>3</v>
       </c>
       <c r="C43" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.35">
@@ -855,7 +855,7 @@
         <v>2</v>
       </c>
       <c r="C44" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.35">
@@ -866,7 +866,7 @@
         <v>2</v>
       </c>
       <c r="C45" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.35">

</xml_diff>